<commit_message>
Refactored the entire code
</commit_message>
<xml_diff>
--- a/SampleQuestions_Mistral.xlsx
+++ b/SampleQuestions_Mistral.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurentiuoprita\Downloads\BATTLE\BATTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurentiuoprita\IdeaProjects\wolf-brigade-aib-2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793D8FB2-6ADD-420C-BEBF-2A3A29E6F732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0210E8BD-61E7-49F0-9DD3-411AA73C0916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>https://chat.mistral.ai/chat</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>what is the speed of light?</t>
+  </si>
+  <si>
+    <t>Expected Answer</t>
   </si>
   <si>
     <t>The hardest natural substance on Earth is diamond. Diamonds are composed of carbon atoms arranged in a specific crystal structure called a diamond cubic, which gives them their exceptional hardness and strength. On the Mohs scale of mineral hardness, diamond is rated as a 10, which is the highest rating. This extreme hardness makes diamonds highly valued for both their aesthetic beauty in jewelry and their industrial applications, such as in cutting tools and abrasives.</t>
@@ -212,9 +215,6 @@
     <t>50 km/h</t>
   </si>
   <si>
-    <t>JavaScript/HTML/CSS</t>
-  </si>
-  <si>
     <t>100 degrees</t>
   </si>
   <si>
@@ -224,37 +224,34 @@
     <t>World War I</t>
   </si>
   <si>
-    <t>attention/careful</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>Rendering/Navigation/Interaction</t>
-  </si>
-  <si>
-    <t>Cacti/Cactuses</t>
-  </si>
-  <si>
-    <t>nucleus/DNA</t>
-  </si>
-  <si>
-    <t>299,792,458</t>
-  </si>
-  <si>
     <t>Keyword</t>
   </si>
   <si>
     <t>Text Matching</t>
   </si>
   <si>
-    <t>CompareByKeywords</t>
-  </si>
-  <si>
-    <t>ExpectedAnswer</t>
-  </si>
-  <si>
-    <t>SimilarityScore (%)</t>
+    <t>Similarity score %</t>
+  </si>
+  <si>
+    <t>JavaScript HTML CSS</t>
+  </si>
+  <si>
+    <t>attention careful</t>
+  </si>
+  <si>
+    <t>Rendering Navigation Interaction</t>
+  </si>
+  <si>
+    <t>Cacti Cactuses</t>
+  </si>
+  <si>
+    <t>nucleus</t>
+  </si>
+  <si>
+    <t>ActualAnswer</t>
   </si>
 </sst>
 </file>
@@ -620,7 +617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -629,7 +628,7 @@
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="6" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -640,22 +639,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -663,10 +662,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -674,10 +673,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -685,10 +684,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -696,10 +695,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -707,10 +706,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -718,10 +717,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -729,10 +728,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -740,10 +739,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -751,10 +750,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="9">
-        <v>3142857</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -765,7 +764,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -773,10 +772,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -784,7 +783,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
@@ -795,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
@@ -806,7 +805,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
         <v>54</v>
@@ -817,10 +816,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -828,10 +827,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="288" x14ac:dyDescent="0.3">
@@ -839,10 +838,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -850,10 +849,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -861,10 +860,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -872,10 +871,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>